<commit_message>
lastest code changes on 26th Nov 2021
</commit_message>
<xml_diff>
--- a/cypress/fixtures/excelFiles/cypressAutomation.xlsx
+++ b/cypress/fixtures/excelFiles/cypressAutomation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d959956\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d959956\Desktop\Projects\Telstra\cypressautomation\cypress\fixtures\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC69B3D-CAD3-4AF4-99E6-ECD56A705D8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABDD41B-EFBF-443D-AE87-0F40D80B9648}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="homePage" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>action</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>homePersonal-Banner-EA</t>
-  </si>
-  <si>
-    <t>visit</t>
   </si>
   <si>
     <t>div[data-personalisation-id='homePersonal-banner-EA']</t>
@@ -615,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -646,10 +643,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="7">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -666,7 +663,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="9" t="str">
         <f>CONCATENATE([1]Sheet_Config!B23,"?livetest=EA_homepage")</f>
@@ -687,12 +684,8 @@
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="11">
-        <v>3</v>
-      </c>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -706,7 +699,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="2"/>
@@ -777,11 +770,11 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>13</v>
@@ -799,7 +792,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="13"/>
     </row>
@@ -808,7 +801,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -819,7 +812,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -838,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57417608-6EDB-45A9-929B-88A8B834A9D9}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -875,7 +868,7 @@
     </row>
     <row r="3" spans="1:5" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="str">
         <f>CONCATENATE([1]Sheet_Config!B23,"/mobile-phones/upgrade-now?livetest=EA_takeover")</f>
@@ -894,7 +887,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -910,7 +903,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -921,7 +914,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="2"/>
@@ -930,7 +923,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="2"/>
@@ -939,7 +932,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="2"/>
@@ -957,7 +950,7 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="2"/>
@@ -968,7 +961,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="2"/>
@@ -976,14 +969,14 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -994,7 +987,7 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1002,7 +995,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1010,7 +1003,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lastest code changes on 2nd Dec 2021
</commit_message>
<xml_diff>
--- a/cypress/fixtures/excelFiles/cypressAutomation.xlsx
+++ b/cypress/fixtures/excelFiles/cypressAutomation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d959956\Desktop\Projects\Telstra\cypressautomation\cypress\fixtures\excelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d959956\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABDD41B-EFBF-443D-AE87-0F40D80B9648}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97DD951-D153-4247-A96C-7896C0CE7910}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>action</t>
   </si>
@@ -70,18 +70,6 @@
     <t>Telstra Personal</t>
   </si>
   <si>
-    <t>This is our test campaign for the capability</t>
-  </si>
-  <si>
-    <t>Join now for your shot at 1 million Telstra Plus points</t>
-  </si>
-  <si>
-    <t>Eligibility criteria apply</t>
-  </si>
-  <si>
-    <t>Learn more</t>
-  </si>
-  <si>
     <t>screenshot</t>
   </si>
   <si>
@@ -97,40 +85,7 @@
     <t>Upgrade now</t>
   </si>
   <si>
-    <t>Join our</t>
-  </si>
-  <si>
-    <t>Join now for your shot at 1 million</t>
-  </si>
-  <si>
-    <t>Enrol now</t>
-  </si>
-  <si>
-    <t>upgrade-banner-EA</t>
-  </si>
-  <si>
-    <t>cta</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>div[data-personalisation-id='upgrade-banner-EA']</t>
-  </si>
-  <si>
-    <t>div.HeadingTitle_title-base__3Gth6</t>
-  </si>
-  <si>
-    <t>Telstra Plus</t>
-  </si>
-  <si>
-    <t>div[data-personalisation-id='mobileOnPlan-banner-EA']</t>
-  </si>
-  <si>
-    <t>Mobiles on a plan</t>
-  </si>
-  <si>
-    <t>homePersonal-Banner-EA_cta1</t>
   </si>
   <si>
     <t>upgrade-banner-EA_cta1</t>
@@ -146,7 +101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,12 +160,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -233,7 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -263,7 +212,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -312,29 +260,29 @@
       <sheetName val="Sheet_Config"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
       <sheetData sheetId="23">
         <row r="23">
           <cell r="B23" t="str">
@@ -610,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -643,7 +591,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B2" s="7">
         <v>50</v>
@@ -663,7 +611,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B4" s="9" t="str">
         <f>CONCATENATE([1]Sheet_Config!B23,"?livetest=EA_homepage")</f>
@@ -683,140 +631,43 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:6" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
-      <c r="B9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="8"/>
-      <c r="B11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
-      <c r="B12" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -829,10 +680,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57417608-6EDB-45A9-929B-88A8B834A9D9}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,7 +719,7 @@
     </row>
     <row r="3" spans="1:5" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="str">
         <f>CONCATENATE([1]Sheet_Config!B23,"/mobile-phones/upgrade-now?livetest=EA_takeover")</f>
@@ -887,7 +738,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -903,7 +754,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -914,96 +765,18 @@
         <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>